<commit_message>
third teams time variable
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
+++ b/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
minute by minute datasets
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
+++ b/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
@@ -587,7 +587,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>['Romania', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Romania']</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>['Portugal', 'Northern Ireland']</t>
+          <t>['Northern Ireland', 'Portugal']</t>
         </is>
       </c>
       <c r="P20" t="n">

</xml_diff>

<commit_message>
three and four teams tied
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
+++ b/data/out/wiki/men/fifa/eu/third_teams_df_eu_fifa.xlsx
@@ -668,10 +668,10 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1207,10 +1207,10 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1361,10 +1361,10 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1518,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="Q14" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1595,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="Q15" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1672,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="Q17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1826,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1900,10 +1900,10 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="Q21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -2211,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="Q23" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -2281,14 +2281,14 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Portugal']</t>
+          <t>['Portugal', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="P24" t="n">
         <v>1</v>
       </c>
       <c r="Q24" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -2365,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="Q25" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="Q27" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
@@ -2673,7 +2673,7 @@
         <v>1</v>
       </c>
       <c r="Q29" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -2750,7 +2750,7 @@
         <v>1</v>
       </c>
       <c r="Q30" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
@@ -2827,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="Q31" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -2904,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="Q32" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
@@ -3058,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="Q34" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
@@ -3671,10 +3671,10 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="Q43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -3828,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="Q44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="Q45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="Q46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="Q47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -4133,10 +4133,10 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -4210,10 +4210,10 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -4290,7 +4290,7 @@
         <v>1</v>
       </c>
       <c r="Q50" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -4364,10 +4364,10 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52">
@@ -4441,10 +4441,10 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q52" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -4521,7 +4521,7 @@
         <v>1</v>
       </c>
       <c r="Q53" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -4598,7 +4598,7 @@
         <v>1</v>
       </c>
       <c r="Q54" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -4675,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="Q55" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -4752,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="Q56" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -4829,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="Q57" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
@@ -4906,7 +4906,7 @@
         <v>1</v>
       </c>
       <c r="Q58" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
@@ -4983,7 +4983,7 @@
         <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
@@ -5060,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="Q60" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61">
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="Q61" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
@@ -5214,7 +5214,7 @@
         <v>1</v>
       </c>
       <c r="Q62" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
@@ -5291,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="Q63" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64">
@@ -5368,7 +5368,7 @@
         <v>1</v>
       </c>
       <c r="Q64" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
@@ -5442,10 +5442,10 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q65" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66">
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67">
@@ -5599,7 +5599,7 @@
         <v>1</v>
       </c>
       <c r="Q67" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68">
@@ -5676,7 +5676,7 @@
         <v>0</v>
       </c>
       <c r="Q68" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -5753,7 +5753,7 @@
         <v>0</v>
       </c>
       <c r="Q69" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
@@ -5830,7 +5830,7 @@
         <v>0</v>
       </c>
       <c r="Q70" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71">
@@ -5907,7 +5907,7 @@
         <v>0</v>
       </c>
       <c r="Q71" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
@@ -5984,7 +5984,7 @@
         <v>0</v>
       </c>
       <c r="Q72" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73">
@@ -6061,7 +6061,7 @@
         <v>0</v>
       </c>
       <c r="Q73" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74">
@@ -6138,7 +6138,7 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75">
@@ -6215,7 +6215,7 @@
         <v>0</v>
       </c>
       <c r="Q75" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76">
@@ -6289,10 +6289,10 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q76" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77">
@@ -6369,7 +6369,7 @@
         <v>1</v>
       </c>
       <c r="Q77" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78">
@@ -6446,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79">
@@ -6523,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="Q79" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80">
@@ -6600,7 +6600,7 @@
         <v>1</v>
       </c>
       <c r="Q80" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81">
@@ -6677,7 +6677,7 @@
         <v>1</v>
       </c>
       <c r="Q81" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82">
@@ -6754,7 +6754,7 @@
         <v>1</v>
       </c>
       <c r="Q82" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83">
@@ -6831,7 +6831,7 @@
         <v>1</v>
       </c>
       <c r="Q83" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84">
@@ -6908,7 +6908,7 @@
         <v>1</v>
       </c>
       <c r="Q84" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85">
@@ -7059,10 +7059,10 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -7139,7 +7139,7 @@
         <v>0</v>
       </c>
       <c r="Q87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -7216,7 +7216,7 @@
         <v>0</v>
       </c>
       <c r="Q88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -7293,7 +7293,7 @@
         <v>1</v>
       </c>
       <c r="Q89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -7370,7 +7370,7 @@
         <v>1</v>
       </c>
       <c r="Q90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="Q91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -7524,7 +7524,7 @@
         <v>0</v>
       </c>
       <c r="Q92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -7601,7 +7601,7 @@
         <v>1</v>
       </c>
       <c r="Q93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94">
@@ -7678,7 +7678,7 @@
         <v>1</v>
       </c>
       <c r="Q94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95">
@@ -7755,7 +7755,7 @@
         <v>0</v>
       </c>
       <c r="Q95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -7832,7 +7832,7 @@
         <v>1</v>
       </c>
       <c r="Q96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97">
@@ -7909,7 +7909,7 @@
         <v>1</v>
       </c>
       <c r="Q97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
@@ -7986,7 +7986,7 @@
         <v>0</v>
       </c>
       <c r="Q98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
@@ -8063,7 +8063,7 @@
         <v>1</v>
       </c>
       <c r="Q99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100">
@@ -8140,7 +8140,7 @@
         <v>1</v>
       </c>
       <c r="Q100" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101">
@@ -8217,7 +8217,7 @@
         <v>0</v>
       </c>
       <c r="Q101" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102">
@@ -8294,7 +8294,7 @@
         <v>1</v>
       </c>
       <c r="Q102" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103">
@@ -8368,10 +8368,10 @@
         </is>
       </c>
       <c r="P103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q103" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104">
@@ -8441,14 +8441,14 @@
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Slovakia']</t>
+          <t>['Slovakia', 'Slovenia']</t>
         </is>
       </c>
       <c r="P104" t="n">
         <v>0</v>
       </c>
       <c r="Q104" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105">
@@ -8522,10 +8522,10 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q105" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106">
@@ -8599,10 +8599,10 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107">
@@ -8679,7 +8679,7 @@
         <v>1</v>
       </c>
       <c r="Q107" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108">
@@ -8756,7 +8756,7 @@
         <v>1</v>
       </c>
       <c r="Q108" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109">
@@ -8833,7 +8833,7 @@
         <v>1</v>
       </c>
       <c r="Q109" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110">
@@ -8910,7 +8910,7 @@
         <v>1</v>
       </c>
       <c r="Q110" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111">
@@ -8987,7 +8987,7 @@
         <v>1</v>
       </c>
       <c r="Q111" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112">
@@ -9064,7 +9064,7 @@
         <v>0</v>
       </c>
       <c r="Q112" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113">
@@ -9134,14 +9134,14 @@
       </c>
       <c r="O113" t="inlineStr">
         <is>
-          <t>['Georgia', 'Netherlands']</t>
+          <t>['Netherlands', 'Georgia']</t>
         </is>
       </c>
       <c r="P113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q113" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="114">
@@ -9218,7 +9218,7 @@
         <v>1</v>
       </c>
       <c r="Q114" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115">
@@ -9288,14 +9288,14 @@
       </c>
       <c r="O115" t="inlineStr">
         <is>
-          <t>['Georgia', 'Netherlands']</t>
+          <t>['Netherlands', 'Georgia']</t>
         </is>
       </c>
       <c r="P115" t="n">
         <v>1</v>
       </c>
       <c r="Q115" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>